<commit_message>
#09 - Data rest 테스트
슬라이스 테스트와 통합 테스트 둘 다 구현.

주의: 테스트지만 DB 접근이 일어나고 있으므로 '@Transition' 을 이용해서 테스트 안에서는 롤백 되도록 동작 시킴
</commit_message>
<xml_diff>
--- a/document/게시판api설계.xlsx
+++ b/document/게시판api설계.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\GOYEJIN\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8E91B6-5B57-4756-A5AB-FAA5D38B31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87211F8E-EC11-4188-8361-D921482C7BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{AB383C05-61B0-45BC-B02C-D51562C28E1E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,14 +217,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/articlesComments</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/articlesComments/{article-comment-id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>특정 게시글과 관련된 댓글 리스트 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,18 +225,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/articles/{article-id}/articlesComments</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/articles/{article-id}/Comments</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/articles/{article-id}/articlesComments/{article-comment-id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,6 +266,22 @@
   </si>
   <si>
     <t>/articles/search/hashtag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/articleComments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/articleComments/{article-comment-id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/articles/{article-id}/articleComments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/articles/{article-id}/articleComments/{article-comment-id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -339,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -351,56 +347,50 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -408,20 +398,195 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -433,7 +598,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -443,47 +608,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,7 +1000,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -813,139 +1011,139 @@
     <col min="5" max="5" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="15"/>
-      <c r="B4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="15"/>
-      <c r="B5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="15"/>
-      <c r="B6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="15"/>
-      <c r="B7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="15"/>
-      <c r="B8" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="15"/>
-      <c r="B9" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="16"/>
-      <c r="B10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="12" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E12" t="s">
@@ -953,207 +1151,207 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="15"/>
-      <c r="B14" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="15"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="15"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="15"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="8"/>
+      <c r="B18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="8"/>
+      <c r="B19" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="8"/>
+      <c r="B20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="8"/>
+      <c r="B21" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="8"/>
+      <c r="B22" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="8"/>
+      <c r="B23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="8"/>
+      <c r="B24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="8"/>
+      <c r="B25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="9"/>
+      <c r="B26" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="15"/>
-      <c r="B18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
-      <c r="B19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="15"/>
-      <c r="B20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="15"/>
-      <c r="B21" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="15"/>
-      <c r="B22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="15"/>
-      <c r="B23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="15"/>
-      <c r="B24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="E26" s="24" t="s">
         <v>55</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="15"/>
-      <c r="B25" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="16"/>
-      <c r="B26" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>